<commit_message>
gran crest start book
</commit_message>
<xml_diff>
--- a/gran-crest/checklist.xlsx
+++ b/gran-crest/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Source/japanese-collectors-list/gran-crest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D5A7E-C094-E947-88E5-1E32D2E28AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CB3B78-B3F7-AE4D-B688-65DB0E5DA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="600" windowWidth="25080" windowHeight="15800" xr2:uid="{7DC794EB-D782-484E-B8D9-11B9DA63736A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>year</t>
   </si>
@@ -63,9 +63,6 @@
     <t>グランクレストRPGルールブック 1</t>
   </si>
   <si>
-    <t>Grand Rest RPG Rulebook 1</t>
-  </si>
-  <si>
     <t>Kadokawa</t>
   </si>
   <si>
@@ -75,18 +72,12 @@
     <t>グランクレストRPGルールブック 2</t>
   </si>
   <si>
-    <t>Grand Rest RPG Rulebook 2</t>
-  </si>
-  <si>
     <t>advanced_rulebook.jpg</t>
   </si>
   <si>
     <t>グランクレストRPG サプリメント 上級ルールブック</t>
   </si>
   <si>
-    <t>Grand Crest RPG Supplement Advanced Rulebook</t>
-  </si>
-  <si>
     <t>グランクレストRPG データブック アドバンスフォース</t>
   </si>
   <si>
@@ -99,12 +90,6 @@
     <t>グランクレスト戦記データブック</t>
   </si>
   <si>
-    <t>Grand Crest RPG Data Book Advanced Force</t>
-  </si>
-  <si>
-    <t>Record of Grand Crest War Data Book</t>
-  </si>
-  <si>
     <t>war_data_book.jpg</t>
   </si>
   <si>
@@ -226,6 +211,33 @@
   </si>
   <si>
     <t>Kakedashi Monarch's Demon King Training 2</t>
+  </si>
+  <si>
+    <t>グランクレストスタートブック 1</t>
+  </si>
+  <si>
+    <t>Granrest Start Book 1</t>
+  </si>
+  <si>
+    <t>Grancrest RPG Rulebook 1</t>
+  </si>
+  <si>
+    <t>Grancest RPG Rulebook 2</t>
+  </si>
+  <si>
+    <t>Grancrest RPG Data Book Advanced Force</t>
+  </si>
+  <si>
+    <t>Grancrest RPG Supplement Advanced Rulebook</t>
+  </si>
+  <si>
+    <t>Record of Grancrest War Data Book</t>
+  </si>
+  <si>
+    <t>start_book.jpg</t>
+  </si>
+  <si>
+    <t>Fujimi Shobo</t>
   </si>
 </sst>
 </file>
@@ -583,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58A2410-0CA7-5C45-A5DA-946C434AA2E6}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="A1:F19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,10 +636,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -641,36 +653,36 @@
         <v>2013</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -681,19 +693,19 @@
         <v>2014</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -701,19 +713,19 @@
         <v>2014</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -721,19 +733,19 @@
         <v>2014</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -741,19 +753,19 @@
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -761,19 +773,19 @@
         <v>2014</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -781,19 +793,19 @@
         <v>2014</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -801,19 +813,19 @@
         <v>2014</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -821,39 +833,39 @@
         <v>2014</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -861,19 +873,19 @@
         <v>2015</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -881,19 +893,19 @@
         <v>2015</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -901,19 +913,19 @@
         <v>2015</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -921,19 +933,19 @@
         <v>2015</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -941,19 +953,19 @@
         <v>2015</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -961,24 +973,44 @@
         <v>2015</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2015</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
-    <sortCondition ref="A2:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
+    <sortCondition ref="A2:A20"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>